<commit_message>
fixed more duplicate names in la liga
</commit_message>
<xml_diff>
--- a/data/league_data/england/20/england_std.xlsx
+++ b/data/league_data/england/20/england_std.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanjitvarma/Desktop/trial_git/Predicting-Football-Player-Transfer-Values/data/league_data/england/20/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0AD0BEDD-E801-2E4F-9C12-A9850C835DCA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{937CFD0D-561C-C74E-9807-8786F2EADA5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14700"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -1375,9 +1375,6 @@
     <t>Ryan Sessegnon</t>
   </si>
   <si>
-    <t>Jota</t>
-  </si>
-  <si>
     <t>Alireza Jahanbakhsh</t>
   </si>
   <si>
@@ -1616,12 +1613,15 @@
   </si>
   <si>
     <t>Angel Gomes</t>
+  </si>
+  <si>
+    <t>Jota Peleteiro</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -2479,11 +2479,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA500"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AC11" sqref="AC11"/>
+    <sheetView tabSelected="1" topLeftCell="A399" workbookViewId="0">
+      <selection activeCell="A414" sqref="A414"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -36793,7 +36793,7 @@
     </row>
     <row r="414" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A414" s="2" t="s">
-        <v>451</v>
+        <v>531</v>
       </c>
       <c r="B414" s="2" t="s">
         <v>61</v>
@@ -36959,7 +36959,7 @@
     </row>
     <row r="416" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A416" s="2" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B416" s="2" t="s">
         <v>41</v>
@@ -37042,7 +37042,7 @@
     </row>
     <row r="417" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A417" s="2" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B417" s="2" t="s">
         <v>35</v>
@@ -37125,7 +37125,7 @@
     </row>
     <row r="418" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A418" s="2" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B418" s="2" t="s">
         <v>23</v>
@@ -37208,7 +37208,7 @@
     </row>
     <row r="419" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A419" s="2" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B419" s="2" t="s">
         <v>43</v>
@@ -37291,7 +37291,7 @@
     </row>
     <row r="420" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A420" s="2" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B420" s="2" t="s">
         <v>35</v>
@@ -37374,7 +37374,7 @@
     </row>
     <row r="421" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A421" s="2" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B421" s="2" t="s">
         <v>23</v>
@@ -37457,7 +37457,7 @@
     </row>
     <row r="422" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A422" s="2" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B422" s="2" t="s">
         <v>46</v>
@@ -37540,7 +37540,7 @@
     </row>
     <row r="423" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A423" s="2" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B423" s="2" t="s">
         <v>53</v>
@@ -37623,7 +37623,7 @@
     </row>
     <row r="424" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A424" s="2" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B424" s="2" t="s">
         <v>39</v>
@@ -37706,7 +37706,7 @@
     </row>
     <row r="425" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A425" s="2" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B425" s="2" t="s">
         <v>72</v>
@@ -37789,7 +37789,7 @@
     </row>
     <row r="426" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A426" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B426" s="2" t="s">
         <v>43</v>
@@ -37872,7 +37872,7 @@
     </row>
     <row r="427" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A427" s="2" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B427" s="2" t="s">
         <v>61</v>
@@ -37955,7 +37955,7 @@
     </row>
     <row r="428" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A428" s="2" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B428" s="2" t="s">
         <v>21</v>
@@ -38038,7 +38038,7 @@
     </row>
     <row r="429" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A429" s="2" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B429" s="2" t="s">
         <v>25</v>
@@ -38204,7 +38204,7 @@
     </row>
     <row r="431" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A431" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B431" s="2" t="s">
         <v>21</v>
@@ -38287,7 +38287,7 @@
     </row>
     <row r="432" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A432" s="2" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B432" s="2" t="s">
         <v>51</v>
@@ -38453,7 +38453,7 @@
     </row>
     <row r="434" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A434" s="2" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B434" s="2" t="s">
         <v>64</v>
@@ -38536,7 +38536,7 @@
     </row>
     <row r="435" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A435" s="2" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B435" s="2" t="s">
         <v>51</v>
@@ -38619,7 +38619,7 @@
     </row>
     <row r="436" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A436" s="2" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B436" s="2" t="s">
         <v>25</v>
@@ -38702,7 +38702,7 @@
     </row>
     <row r="437" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A437" s="2" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B437" s="2" t="s">
         <v>56</v>
@@ -38785,7 +38785,7 @@
     </row>
     <row r="438" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A438" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B438" s="2" t="s">
         <v>39</v>
@@ -38868,7 +38868,7 @@
     </row>
     <row r="439" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A439" s="2" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B439" s="2" t="s">
         <v>27</v>
@@ -38951,7 +38951,7 @@
     </row>
     <row r="440" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A440" s="2" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B440" s="2" t="s">
         <v>64</v>
@@ -39034,7 +39034,7 @@
     </row>
     <row r="441" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A441" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B441" s="2" t="s">
         <v>61</v>
@@ -39117,7 +39117,7 @@
     </row>
     <row r="442" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A442" s="2" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B442" s="2" t="s">
         <v>53</v>
@@ -39200,7 +39200,7 @@
     </row>
     <row r="443" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A443" s="2" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B443" s="2" t="s">
         <v>64</v>
@@ -39283,7 +39283,7 @@
     </row>
     <row r="444" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A444" s="2" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B444" s="2" t="s">
         <v>31</v>
@@ -39366,7 +39366,7 @@
     </row>
     <row r="445" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A445" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B445" s="2" t="s">
         <v>23</v>
@@ -39449,7 +39449,7 @@
     </row>
     <row r="446" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A446" s="2" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B446" s="2" t="s">
         <v>25</v>
@@ -39532,7 +39532,7 @@
     </row>
     <row r="447" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A447" s="2" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B447" s="2" t="s">
         <v>21</v>
@@ -39615,7 +39615,7 @@
     </row>
     <row r="448" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A448" s="2" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B448" s="2" t="s">
         <v>39</v>
@@ -39698,7 +39698,7 @@
     </row>
     <row r="449" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A449" s="2" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B449" s="2" t="s">
         <v>53</v>
@@ -39781,7 +39781,7 @@
     </row>
     <row r="450" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A450" s="2" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B450" s="2" t="s">
         <v>23</v>
@@ -39864,7 +39864,7 @@
     </row>
     <row r="451" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A451" s="2" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B451" s="2" t="s">
         <v>56</v>
@@ -39947,7 +39947,7 @@
     </row>
     <row r="452" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A452" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B452" s="2" t="s">
         <v>31</v>
@@ -40030,7 +40030,7 @@
     </row>
     <row r="453" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A453" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B453" s="2" t="s">
         <v>39</v>
@@ -40113,7 +40113,7 @@
     </row>
     <row r="454" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A454" s="2" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B454" s="2" t="s">
         <v>27</v>
@@ -40196,7 +40196,7 @@
     </row>
     <row r="455" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A455" s="2" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B455" s="2" t="s">
         <v>31</v>
@@ -40279,7 +40279,7 @@
     </row>
     <row r="456" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A456" s="2" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B456" s="2" t="s">
         <v>35</v>
@@ -40362,7 +40362,7 @@
     </row>
     <row r="457" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A457" s="2" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B457" s="2" t="s">
         <v>31</v>
@@ -40445,7 +40445,7 @@
     </row>
     <row r="458" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A458" s="2" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B458" s="2" t="s">
         <v>23</v>
@@ -40528,7 +40528,7 @@
     </row>
     <row r="459" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A459" s="2" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B459" s="2" t="s">
         <v>51</v>
@@ -40611,7 +40611,7 @@
     </row>
     <row r="460" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A460" s="2" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B460" s="2" t="s">
         <v>25</v>
@@ -40694,7 +40694,7 @@
     </row>
     <row r="461" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A461" s="2" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B461" s="2" t="s">
         <v>31</v>
@@ -40777,7 +40777,7 @@
     </row>
     <row r="462" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A462" s="2" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B462" s="2" t="s">
         <v>61</v>
@@ -40860,7 +40860,7 @@
     </row>
     <row r="463" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A463" s="2" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B463" s="2" t="s">
         <v>39</v>
@@ -40943,7 +40943,7 @@
     </row>
     <row r="464" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A464" s="2" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B464" s="2" t="s">
         <v>72</v>
@@ -41026,7 +41026,7 @@
     </row>
     <row r="465" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A465" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B465" s="2" t="s">
         <v>72</v>
@@ -41109,7 +41109,7 @@
     </row>
     <row r="466" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A466" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B466" s="2" t="s">
         <v>21</v>
@@ -41192,7 +41192,7 @@
     </row>
     <row r="467" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A467" s="2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B467" s="2" t="s">
         <v>39</v>
@@ -41275,7 +41275,7 @@
     </row>
     <row r="468" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A468" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B468" s="2" t="s">
         <v>31</v>
@@ -41358,7 +41358,7 @@
     </row>
     <row r="469" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A469" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B469" s="2" t="s">
         <v>72</v>
@@ -41441,7 +41441,7 @@
     </row>
     <row r="470" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A470" s="2" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B470" s="2" t="s">
         <v>53</v>
@@ -41524,7 +41524,7 @@
     </row>
     <row r="471" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A471" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B471" s="2" t="s">
         <v>51</v>
@@ -41607,7 +41607,7 @@
     </row>
     <row r="472" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A472" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B472" s="2" t="s">
         <v>46</v>
@@ -41690,7 +41690,7 @@
     </row>
     <row r="473" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A473" s="2" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B473" s="2" t="s">
         <v>41</v>
@@ -41773,7 +41773,7 @@
     </row>
     <row r="474" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A474" s="2" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B474" s="2" t="s">
         <v>92</v>
@@ -41856,7 +41856,7 @@
     </row>
     <row r="475" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A475" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B475" s="2" t="s">
         <v>29</v>
@@ -41939,7 +41939,7 @@
     </row>
     <row r="476" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A476" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B476" s="2" t="s">
         <v>41</v>
@@ -42022,7 +42022,7 @@
     </row>
     <row r="477" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A477" s="2" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B477" s="2" t="s">
         <v>29</v>
@@ -42105,7 +42105,7 @@
     </row>
     <row r="478" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A478" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B478" s="2" t="s">
         <v>92</v>
@@ -42188,7 +42188,7 @@
     </row>
     <row r="479" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A479" s="2" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B479" s="2" t="s">
         <v>92</v>
@@ -42271,7 +42271,7 @@
     </row>
     <row r="480" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A480" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B480" s="2" t="s">
         <v>31</v>
@@ -42354,7 +42354,7 @@
     </row>
     <row r="481" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A481" s="2" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B481" s="2" t="s">
         <v>41</v>
@@ -42437,7 +42437,7 @@
     </row>
     <row r="482" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A482" s="2" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B482" s="2" t="s">
         <v>29</v>
@@ -42520,7 +42520,7 @@
     </row>
     <row r="483" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A483" s="2" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B483" s="2" t="s">
         <v>37</v>
@@ -42603,7 +42603,7 @@
     </row>
     <row r="484" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A484" s="2" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B484" s="2" t="s">
         <v>29</v>
@@ -42686,7 +42686,7 @@
     </row>
     <row r="485" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A485" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B485" s="2" t="s">
         <v>61</v>
@@ -42769,7 +42769,7 @@
     </row>
     <row r="486" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A486" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B486" s="2" t="s">
         <v>51</v>
@@ -42852,7 +42852,7 @@
     </row>
     <row r="487" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A487" s="2" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B487" s="2" t="s">
         <v>56</v>
@@ -42935,7 +42935,7 @@
     </row>
     <row r="488" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A488" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B488" s="2" t="s">
         <v>31</v>
@@ -43018,7 +43018,7 @@
     </row>
     <row r="489" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A489" s="2" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B489" s="2" t="s">
         <v>56</v>
@@ -43101,7 +43101,7 @@
     </row>
     <row r="490" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A490" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B490" s="2" t="s">
         <v>21</v>
@@ -43184,7 +43184,7 @@
     </row>
     <row r="491" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A491" s="2" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B491" s="2" t="s">
         <v>39</v>
@@ -43350,7 +43350,7 @@
     </row>
     <row r="493" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A493" s="2" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B493" s="2" t="s">
         <v>51</v>
@@ -43433,7 +43433,7 @@
     </row>
     <row r="494" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A494" s="2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B494" s="2" t="s">
         <v>56</v>
@@ -43516,7 +43516,7 @@
     </row>
     <row r="495" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A495" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B495" s="2" t="s">
         <v>29</v>
@@ -43599,7 +43599,7 @@
     </row>
     <row r="496" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A496" s="2" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B496" s="2" t="s">
         <v>92</v>
@@ -43682,7 +43682,7 @@
     </row>
     <row r="497" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A497" s="2" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B497" s="2" t="s">
         <v>35</v>
@@ -43765,7 +43765,7 @@
     </row>
     <row r="498" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A498" s="2" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B498" s="2" t="s">
         <v>29</v>
@@ -43848,7 +43848,7 @@
     </row>
     <row r="499" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A499" s="2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B499" s="2" t="s">
         <v>56</v>
@@ -43931,7 +43931,7 @@
     </row>
     <row r="500" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A500" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B500" s="2" t="s">
         <v>31</v>

</xml_diff>